<commit_message>
Completed the functions table
</commit_message>
<xml_diff>
--- a/Back End Functions List.xlsx
+++ b/Back End Functions List.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D9ADAEA-3C86-4CD8-8420-725ECA8556CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pulki\Desktop\PULKIT\School\Year 3\Sem 2\SQA\backend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFCF4FD-CF7A-4BE7-849B-2584630B013F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>Class</t>
   </si>
@@ -187,13 +192,40 @@
   </si>
   <si>
     <t>gets the buyer name listed as UUUU... in the requirements doc if there is one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readFile(String filename) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads strings from given file (filename) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">getUsers(ArrayList&lt;String&gt; userStrings) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">getItems(ArrayList&lt;String&gt;itemStrings) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">takes in an ArrayList of Strings and builds an ArrayList&lt;Items&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">takes in an ArrayList of Strings and builds an ArrayList&lt;Users&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">writeToFile(ArrayList&lt;String&gt; strings, String filename) </t>
+  </si>
+  <si>
+    <t>writes Strings from ArrayList: strings to file: filename</t>
+  </si>
+  <si>
+    <t>Driver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,20 +579,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
     <col min="3" max="3" width="71.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -582,7 +614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -593,7 +625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -604,7 +636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -615,7 +647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -626,7 +658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -637,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -648,7 +680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -659,7 +691,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -670,7 +702,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -681,7 +713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -692,7 +724,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -703,7 +735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -714,7 +746,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -725,7 +757,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -736,7 +768,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -747,7 +779,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -758,7 +790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -769,7 +801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -780,7 +812,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -791,7 +823,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -802,7 +834,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -813,7 +845,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -824,7 +856,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -835,7 +867,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -844,6 +876,50 @@
       </c>
       <c r="C26" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>